<commit_message>
Edit to Excel forms
6 to 3 decimals
</commit_message>
<xml_diff>
--- a/Form_DLM_SurveyReport.xlsx
+++ b/Form_DLM_SurveyReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Assembly-Survey-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58746F5B-B0B0-413C-9F68-11F369478739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B74BDF-61AF-4C69-AB22-071985B6A240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,6 +947,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -958,9 +961,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1312,7 +1312,7 @@
   <dimension ref="B1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1597,15 +1597,15 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F36" s="80" t="e">
+      <c r="F36" s="76" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G36" s="80" t="e">
+      <c r="G36" s="76" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H36" s="80" t="e">
+      <c r="H36" s="76" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -1683,11 +1683,11 @@
       <c r="B42" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="76" t="s">
+      <c r="C42" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="77"/>
-      <c r="E42" s="78"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="79"/>
       <c r="F42" s="41"/>
       <c r="G42" s="42"/>
       <c r="H42" s="43"/>
@@ -2457,11 +2457,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="210" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="79"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="27"/>
@@ -2590,21 +2590,21 @@
       <c r="B23" s="25"/>
     </row>
     <row r="24" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="79"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="79"/>
-      <c r="O24" s="79"/>
+      <c r="A24" s="80"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="27"/>
@@ -3712,11 +3712,11 @@
       <c r="O89" s="25"/>
     </row>
     <row r="90" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="79"/>
-      <c r="B90" s="79"/>
-      <c r="C90" s="79"/>
-      <c r="D90" s="79"/>
-      <c r="E90" s="79"/>
+      <c r="A90" s="80"/>
+      <c r="B90" s="80"/>
+      <c r="C90" s="80"/>
+      <c r="D90" s="80"/>
+      <c r="E90" s="80"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="27"/>
@@ -3845,21 +3845,21 @@
       <c r="B112" s="25"/>
     </row>
     <row r="113" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="79"/>
-      <c r="B113" s="79"/>
-      <c r="C113" s="79"/>
-      <c r="D113" s="79"/>
-      <c r="E113" s="79"/>
-      <c r="F113" s="79"/>
-      <c r="G113" s="79"/>
-      <c r="H113" s="79"/>
-      <c r="I113" s="79"/>
-      <c r="J113" s="79"/>
-      <c r="K113" s="79"/>
-      <c r="L113" s="79"/>
-      <c r="M113" s="79"/>
-      <c r="N113" s="79"/>
-      <c r="O113" s="79"/>
+      <c r="A113" s="80"/>
+      <c r="B113" s="80"/>
+      <c r="C113" s="80"/>
+      <c r="D113" s="80"/>
+      <c r="E113" s="80"/>
+      <c r="F113" s="80"/>
+      <c r="G113" s="80"/>
+      <c r="H113" s="80"/>
+      <c r="I113" s="80"/>
+      <c r="J113" s="80"/>
+      <c r="K113" s="80"/>
+      <c r="L113" s="80"/>
+      <c r="M113" s="80"/>
+      <c r="N113" s="80"/>
+      <c r="O113" s="80"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="27"/>
@@ -4015,11 +4015,11 @@
       <c r="O122" s="25"/>
     </row>
     <row r="123" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="79"/>
-      <c r="B123" s="79"/>
-      <c r="C123" s="79"/>
-      <c r="D123" s="79"/>
-      <c r="E123" s="79"/>
+      <c r="A123" s="80"/>
+      <c r="B123" s="80"/>
+      <c r="C123" s="80"/>
+      <c r="D123" s="80"/>
+      <c r="E123" s="80"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A124" s="27"/>
@@ -4148,21 +4148,21 @@
       <c r="B145" s="25"/>
     </row>
     <row r="146" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="79"/>
-      <c r="B146" s="79"/>
-      <c r="C146" s="79"/>
-      <c r="D146" s="79"/>
-      <c r="E146" s="79"/>
-      <c r="F146" s="79"/>
-      <c r="G146" s="79"/>
-      <c r="H146" s="79"/>
-      <c r="I146" s="79"/>
-      <c r="J146" s="79"/>
-      <c r="K146" s="79"/>
-      <c r="L146" s="79"/>
-      <c r="M146" s="79"/>
-      <c r="N146" s="79"/>
-      <c r="O146" s="79"/>
+      <c r="A146" s="80"/>
+      <c r="B146" s="80"/>
+      <c r="C146" s="80"/>
+      <c r="D146" s="80"/>
+      <c r="E146" s="80"/>
+      <c r="F146" s="80"/>
+      <c r="G146" s="80"/>
+      <c r="H146" s="80"/>
+      <c r="I146" s="80"/>
+      <c r="J146" s="80"/>
+      <c r="K146" s="80"/>
+      <c r="L146" s="80"/>
+      <c r="M146" s="80"/>
+      <c r="N146" s="80"/>
+      <c r="O146" s="80"/>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A147" s="27"/>
@@ -4335,11 +4335,11 @@
       <c r="O156" s="25"/>
     </row>
     <row r="157" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="79"/>
-      <c r="B157" s="79"/>
-      <c r="C157" s="79"/>
-      <c r="D157" s="79"/>
-      <c r="E157" s="79"/>
+      <c r="A157" s="80"/>
+      <c r="B157" s="80"/>
+      <c r="C157" s="80"/>
+      <c r="D157" s="80"/>
+      <c r="E157" s="80"/>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A158" s="27"/>
@@ -4468,21 +4468,21 @@
       <c r="B179" s="25"/>
     </row>
     <row r="180" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="79"/>
-      <c r="B180" s="79"/>
-      <c r="C180" s="79"/>
-      <c r="D180" s="79"/>
-      <c r="E180" s="79"/>
-      <c r="F180" s="79"/>
-      <c r="G180" s="79"/>
-      <c r="H180" s="79"/>
-      <c r="I180" s="79"/>
-      <c r="J180" s="79"/>
-      <c r="K180" s="79"/>
-      <c r="L180" s="79"/>
-      <c r="M180" s="79"/>
-      <c r="N180" s="79"/>
-      <c r="O180" s="79"/>
+      <c r="A180" s="80"/>
+      <c r="B180" s="80"/>
+      <c r="C180" s="80"/>
+      <c r="D180" s="80"/>
+      <c r="E180" s="80"/>
+      <c r="F180" s="80"/>
+      <c r="G180" s="80"/>
+      <c r="H180" s="80"/>
+      <c r="I180" s="80"/>
+      <c r="J180" s="80"/>
+      <c r="K180" s="80"/>
+      <c r="L180" s="80"/>
+      <c r="M180" s="80"/>
+      <c r="N180" s="80"/>
+      <c r="O180" s="80"/>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A181" s="27"/>
@@ -4621,11 +4621,11 @@
       <c r="O188" s="25"/>
     </row>
     <row r="189" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="79"/>
-      <c r="B189" s="79"/>
-      <c r="C189" s="79"/>
-      <c r="D189" s="79"/>
-      <c r="E189" s="79"/>
+      <c r="A189" s="80"/>
+      <c r="B189" s="80"/>
+      <c r="C189" s="80"/>
+      <c r="D189" s="80"/>
+      <c r="E189" s="80"/>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A190" s="27"/>
@@ -4754,21 +4754,21 @@
       <c r="B211" s="25"/>
     </row>
     <row r="212" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="79"/>
-      <c r="B212" s="79"/>
-      <c r="C212" s="79"/>
-      <c r="D212" s="79"/>
-      <c r="E212" s="79"/>
-      <c r="F212" s="79"/>
-      <c r="G212" s="79"/>
-      <c r="H212" s="79"/>
-      <c r="I212" s="79"/>
-      <c r="J212" s="79"/>
-      <c r="K212" s="79"/>
-      <c r="L212" s="79"/>
-      <c r="M212" s="79"/>
-      <c r="N212" s="79"/>
-      <c r="O212" s="79"/>
+      <c r="A212" s="80"/>
+      <c r="B212" s="80"/>
+      <c r="C212" s="80"/>
+      <c r="D212" s="80"/>
+      <c r="E212" s="80"/>
+      <c r="F212" s="80"/>
+      <c r="G212" s="80"/>
+      <c r="H212" s="80"/>
+      <c r="I212" s="80"/>
+      <c r="J212" s="80"/>
+      <c r="K212" s="80"/>
+      <c r="L212" s="80"/>
+      <c r="M212" s="80"/>
+      <c r="N212" s="80"/>
+      <c r="O212" s="80"/>
     </row>
     <row r="213" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A213" s="27"/>
@@ -4924,11 +4924,11 @@
       <c r="O221" s="25"/>
     </row>
     <row r="222" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A222" s="79"/>
-      <c r="B222" s="79"/>
-      <c r="C222" s="79"/>
-      <c r="D222" s="79"/>
-      <c r="E222" s="79"/>
+      <c r="A222" s="80"/>
+      <c r="B222" s="80"/>
+      <c r="C222" s="80"/>
+      <c r="D222" s="80"/>
+      <c r="E222" s="80"/>
     </row>
     <row r="223" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A223" s="27"/>
@@ -5057,21 +5057,21 @@
       <c r="B244" s="25"/>
     </row>
     <row r="245" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A245" s="79"/>
-      <c r="B245" s="79"/>
-      <c r="C245" s="79"/>
-      <c r="D245" s="79"/>
-      <c r="E245" s="79"/>
-      <c r="F245" s="79"/>
-      <c r="G245" s="79"/>
-      <c r="H245" s="79"/>
-      <c r="I245" s="79"/>
-      <c r="J245" s="79"/>
-      <c r="K245" s="79"/>
-      <c r="L245" s="79"/>
-      <c r="M245" s="79"/>
-      <c r="N245" s="79"/>
-      <c r="O245" s="79"/>
+      <c r="A245" s="80"/>
+      <c r="B245" s="80"/>
+      <c r="C245" s="80"/>
+      <c r="D245" s="80"/>
+      <c r="E245" s="80"/>
+      <c r="F245" s="80"/>
+      <c r="G245" s="80"/>
+      <c r="H245" s="80"/>
+      <c r="I245" s="80"/>
+      <c r="J245" s="80"/>
+      <c r="K245" s="80"/>
+      <c r="L245" s="80"/>
+      <c r="M245" s="80"/>
+      <c r="N245" s="80"/>
+      <c r="O245" s="80"/>
     </row>
     <row r="246" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A246" s="27"/>
@@ -5227,11 +5227,11 @@
       <c r="O254" s="25"/>
     </row>
     <row r="255" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A255" s="79"/>
-      <c r="B255" s="79"/>
-      <c r="C255" s="79"/>
-      <c r="D255" s="79"/>
-      <c r="E255" s="79"/>
+      <c r="A255" s="80"/>
+      <c r="B255" s="80"/>
+      <c r="C255" s="80"/>
+      <c r="D255" s="80"/>
+      <c r="E255" s="80"/>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A256" s="27"/>
@@ -5360,21 +5360,21 @@
       <c r="B277" s="25"/>
     </row>
     <row r="278" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A278" s="79"/>
-      <c r="B278" s="79"/>
-      <c r="C278" s="79"/>
-      <c r="D278" s="79"/>
-      <c r="E278" s="79"/>
-      <c r="F278" s="79"/>
-      <c r="G278" s="79"/>
-      <c r="H278" s="79"/>
-      <c r="I278" s="79"/>
-      <c r="J278" s="79"/>
-      <c r="K278" s="79"/>
-      <c r="L278" s="79"/>
-      <c r="M278" s="79"/>
-      <c r="N278" s="79"/>
-      <c r="O278" s="79"/>
+      <c r="A278" s="80"/>
+      <c r="B278" s="80"/>
+      <c r="C278" s="80"/>
+      <c r="D278" s="80"/>
+      <c r="E278" s="80"/>
+      <c r="F278" s="80"/>
+      <c r="G278" s="80"/>
+      <c r="H278" s="80"/>
+      <c r="I278" s="80"/>
+      <c r="J278" s="80"/>
+      <c r="K278" s="80"/>
+      <c r="L278" s="80"/>
+      <c r="M278" s="80"/>
+      <c r="N278" s="80"/>
+      <c r="O278" s="80"/>
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A279" s="27"/>
@@ -5530,11 +5530,11 @@
       <c r="O287" s="25"/>
     </row>
     <row r="288" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A288" s="79"/>
-      <c r="B288" s="79"/>
-      <c r="C288" s="79"/>
-      <c r="D288" s="79"/>
-      <c r="E288" s="79"/>
+      <c r="A288" s="80"/>
+      <c r="B288" s="80"/>
+      <c r="C288" s="80"/>
+      <c r="D288" s="80"/>
+      <c r="E288" s="80"/>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="27"/>
@@ -5663,21 +5663,21 @@
       <c r="B310" s="25"/>
     </row>
     <row r="311" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A311" s="79"/>
-      <c r="B311" s="79"/>
-      <c r="C311" s="79"/>
-      <c r="D311" s="79"/>
-      <c r="E311" s="79"/>
-      <c r="F311" s="79"/>
-      <c r="G311" s="79"/>
-      <c r="H311" s="79"/>
-      <c r="I311" s="79"/>
-      <c r="J311" s="79"/>
-      <c r="K311" s="79"/>
-      <c r="L311" s="79"/>
-      <c r="M311" s="79"/>
-      <c r="N311" s="79"/>
-      <c r="O311" s="79"/>
+      <c r="A311" s="80"/>
+      <c r="B311" s="80"/>
+      <c r="C311" s="80"/>
+      <c r="D311" s="80"/>
+      <c r="E311" s="80"/>
+      <c r="F311" s="80"/>
+      <c r="G311" s="80"/>
+      <c r="H311" s="80"/>
+      <c r="I311" s="80"/>
+      <c r="J311" s="80"/>
+      <c r="K311" s="80"/>
+      <c r="L311" s="80"/>
+      <c r="M311" s="80"/>
+      <c r="N311" s="80"/>
+      <c r="O311" s="80"/>
     </row>
     <row r="312" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A312" s="27"/>
@@ -5833,11 +5833,11 @@
       <c r="O320" s="25"/>
     </row>
     <row r="321" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A321" s="79"/>
-      <c r="B321" s="79"/>
-      <c r="C321" s="79"/>
-      <c r="D321" s="79"/>
-      <c r="E321" s="79"/>
+      <c r="A321" s="80"/>
+      <c r="B321" s="80"/>
+      <c r="C321" s="80"/>
+      <c r="D321" s="80"/>
+      <c r="E321" s="80"/>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="27"/>
@@ -5966,21 +5966,21 @@
       <c r="B343" s="25"/>
     </row>
     <row r="344" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A344" s="79"/>
-      <c r="B344" s="79"/>
-      <c r="C344" s="79"/>
-      <c r="D344" s="79"/>
-      <c r="E344" s="79"/>
-      <c r="F344" s="79"/>
-      <c r="G344" s="79"/>
-      <c r="H344" s="79"/>
-      <c r="I344" s="79"/>
-      <c r="J344" s="79"/>
-      <c r="K344" s="79"/>
-      <c r="L344" s="79"/>
-      <c r="M344" s="79"/>
-      <c r="N344" s="79"/>
-      <c r="O344" s="79"/>
+      <c r="A344" s="80"/>
+      <c r="B344" s="80"/>
+      <c r="C344" s="80"/>
+      <c r="D344" s="80"/>
+      <c r="E344" s="80"/>
+      <c r="F344" s="80"/>
+      <c r="G344" s="80"/>
+      <c r="H344" s="80"/>
+      <c r="I344" s="80"/>
+      <c r="J344" s="80"/>
+      <c r="K344" s="80"/>
+      <c r="L344" s="80"/>
+      <c r="M344" s="80"/>
+      <c r="N344" s="80"/>
+      <c r="O344" s="80"/>
     </row>
     <row r="345" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A345" s="27"/>
@@ -6813,16 +6813,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="79"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>

</xml_diff>